<commit_message>
add some new commands to excel and add title to hello.html
</commit_message>
<xml_diff>
--- a/Git commands.xlsx
+++ b/Git commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zheny\Documents\USB_SIUSKO\LERN PYTHON\P_WEB\lecture_1_Git\hello\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327EC835-B7F0-4AFD-912E-88E43458850F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E21B20-95A2-4271-AF92-F7C6D05F7B84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13650" yWindow="2550" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2550" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Command</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>it should be done before any commits</t>
+  </si>
+  <si>
+    <t>am means git commit all of the files that have been changed--</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git commit -am "text abou commit" </t>
   </si>
 </sst>
 </file>
@@ -481,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -535,121 +541,129 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="25.5">
-      <c r="A7" s="3" t="s">
+    <row r="8" spans="1:2">
+      <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="25.5">
-      <c r="A8" s="3" t="s">
+    <row r="9" spans="1:2">
+      <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="25.5">
-      <c r="A9" s="3" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="25.5">
-      <c r="A10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="25.5">
-      <c r="A16" s="3" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="25.5">
-      <c r="A17" s="3" t="s">
+    <row r="18" spans="1:2">
+      <c r="A18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="25.5">
-      <c r="A18" s="3" t="s">
+    <row r="19" spans="1:2">
+      <c r="A19" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="25.5">
-      <c r="A19" s="3" t="s">
+    <row r="20" spans="1:2" ht="25.5">
+      <c r="A20" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="3" t="s">
+    <row r="21" spans="1:2">
+      <c r="A21" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>